<commit_message>
feat: insert data from excel
</commit_message>
<xml_diff>
--- a/ramp-up-project/back-end/upload-service/upload/excelfile.xlsx
+++ b/ramp-up-project/back-end/upload-service/upload/excelfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lakshan\Pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7174577A-7485-4520-A198-C4C944E41B57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94D115B-8A62-4C47-8A25-4E31FA8F4878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA402AB-EC06-47DD-885E-CC392C2FE1B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA402AB-EC06-47DD-885E-CC392C2FE1B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,36 +34,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>row1col1</t>
-  </si>
-  <si>
-    <t>row1col2</t>
-  </si>
-  <si>
-    <t>row1col3</t>
-  </si>
-  <si>
-    <t>row1col4</t>
-  </si>
-  <si>
-    <t>row1col5</t>
-  </si>
-  <si>
-    <t>row2col1</t>
-  </si>
-  <si>
-    <t>row2col2</t>
-  </si>
-  <si>
-    <t>row2col3</t>
-  </si>
-  <si>
-    <t>row2col4</t>
-  </si>
-  <si>
-    <t>row2col5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>car_make</t>
+  </si>
+  <si>
+    <t>car_model</t>
+  </si>
+  <si>
+    <t>vin_number</t>
+  </si>
+  <si>
+    <t>manufactured_date</t>
+  </si>
+  <si>
+    <t>Allister</t>
+  </si>
+  <si>
+    <t>Camili</t>
+  </si>
+  <si>
+    <t>Chegutu</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>3434989GDS</t>
+  </si>
+  <si>
+    <t>Kasper</t>
+  </si>
+  <si>
+    <t>Cogger</t>
+  </si>
+  <si>
+    <t>Caballococha</t>
+  </si>
+  <si>
+    <t>Subaru</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>WE3942948</t>
   </si>
 </sst>
 </file>
@@ -99,8 +129,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,15 +446,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A31B05-280F-449E-BC52-7F8B8E9EE33B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,22 +479,66 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1">
+        <v>32935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1">
+        <v>30740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>